<commit_message>
Added more techs to network, get csp fraction for plt
</commit_message>
<xml_diff>
--- a/input_files/CSP_case.xlsx
+++ b/input_files/CSP_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/m_/v6c97p3x1mg6bmvchddj43dc0000gn/T/fz3temp-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73191B8-8248-E54F-84E8-FC171B52CFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA94ACD-8733-F54B-8BB1-880CCCCCCB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="103">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -269,9 +269,6 @@
     <t>p_max_pu</t>
   </si>
   <si>
-    <t>lost_load</t>
-  </si>
-  <si>
     <t>csp_test</t>
   </si>
   <si>
@@ -281,19 +278,70 @@
     <t>concentrated solar</t>
   </si>
   <si>
-    <t>input_files/updated_costs_orca_base.csv</t>
-  </si>
-  <si>
-    <t>csp-glasspoint</t>
-  </si>
-  <si>
-    <t>380</t>
-  </si>
-  <si>
     <t>2023-01-01 00:00:00</t>
   </si>
   <si>
-    <t>2023-05-31 23:00:00</t>
+    <t>db</t>
+  </si>
+  <si>
+    <t>heat</t>
+  </si>
+  <si>
+    <t>solar</t>
+  </si>
+  <si>
+    <t>gas boiler steam</t>
+  </si>
+  <si>
+    <t>gas boiler</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>electric boiler steam</t>
+  </si>
+  <si>
+    <t>electric boiler</t>
+  </si>
+  <si>
+    <t>molten salt storage</t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>#Link</t>
+  </si>
+  <si>
+    <t>#Store</t>
+  </si>
+  <si>
+    <t>input_files/costs_concentrated_solar.csv</t>
+  </si>
+  <si>
+    <t>Molten-Salt-charger glasspoint</t>
+  </si>
+  <si>
+    <t>Molten-Salt-discharger glasspoint</t>
+  </si>
+  <si>
+    <t>molten salt disbicharger</t>
+  </si>
+  <si>
+    <t>molten salt charger</t>
+  </si>
+  <si>
+    <t>Molten-Salt-store glasspoint</t>
+  </si>
+  <si>
+    <t>solar-utility single-axis tracking</t>
+  </si>
+  <si>
+    <t>csp glasspoint</t>
+  </si>
+  <si>
+    <t>2023-12-31 23:00:00</t>
   </si>
 </sst>
 </file>
@@ -1186,10 +1234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1452,7 +1500,7 @@
         <v>64</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1468,7 +1516,7 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1476,7 +1524,7 @@
         <v>21</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1484,7 +1532,7 @@
         <v>22</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" t="s">
@@ -1496,7 +1544,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C31" s="6"/>
     </row>
@@ -1515,7 +1563,7 @@
       </c>
       <c r="B33" s="11">
         <f>((B31-B30)*24+1)/B32</f>
-        <v>3624.0000000000582</v>
+        <v>8760.0000000000582</v>
       </c>
       <c r="C33" t="s">
         <v>58</v>
@@ -1527,7 +1575,7 @@
       </c>
       <c r="B34" s="11">
         <f>B33*B32</f>
-        <v>3624.0000000000582</v>
+        <v>8760.0000000000582</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
@@ -1683,7 +1731,7 @@
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -1698,89 +1746,240 @@
         <v>30</v>
       </c>
       <c r="B51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" t="s">
         <v>83</v>
       </c>
-      <c r="C51" t="s">
-        <v>81</v>
-      </c>
-      <c r="D51" t="s">
-        <v>72</v>
-      </c>
-      <c r="H51">
-        <v>1</v>
-      </c>
       <c r="I51" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J51" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
-      <c r="K51" s="5">
-        <v>0</v>
+      <c r="K51" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="L51" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
-      <c r="N51" s="5">
-        <v>1</v>
-      </c>
-      <c r="O51" s="5">
-        <v>25</v>
+      <c r="N51" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O51" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C52" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" t="s">
+        <v>83</v>
+      </c>
+      <c r="E52" t="s">
+        <v>91</v>
+      </c>
+      <c r="I52" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O52" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B53" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" t="s">
+        <v>91</v>
+      </c>
+      <c r="I53" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="M53" t="b">
+        <v>1</v>
+      </c>
+      <c r="N53" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O53" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" t="s">
+        <v>83</v>
+      </c>
+      <c r="E54" t="s">
+        <v>91</v>
+      </c>
+      <c r="I54" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="N54" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O54" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B52" t="s">
-        <v>78</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="B55" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" t="s">
+        <v>86</v>
+      </c>
+      <c r="D55" t="s">
+        <v>83</v>
+      </c>
+      <c r="I55" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="N55" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O55" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" t="s">
         <v>72</v>
       </c>
-      <c r="I52" s="15"/>
-      <c r="K52" s="5">
-        <v>10000</v>
-      </c>
-      <c r="L52" t="str">
-        <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
-        <v>$/MWh</v>
-      </c>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="I56" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="K56" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="N56" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O56" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" t="s">
+        <v>83</v>
+      </c>
+      <c r="I57" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="K57" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="N57" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O57" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58" s="6"/>
+      <c r="I58" s="15"/>
+      <c r="K58" s="5"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="10" t="s">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="L58" s="7"/>
-      <c r="M58" s="7"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>55</v>
       </c>
-      <c r="L59" s="7"/>
-      <c r="M59" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>